<commit_message>
BC nhập hàng: thêm cột 'Nhóm hàng'
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoNhapHang/Teamplate_BaoCaoNhapHangChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoNhapHang/Teamplate_BaoCaoNhapHangChiTiet.xlsx
@@ -17,272 +17,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <r>
-      <t xml:space="preserve">Mã chứng từ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Tổng cộng:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Ngày chứng từ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(2)</t>
-    </r>
-  </si>
-  <si>
     <t>BÁO CÁO NHẬP HÀNG CHI TIẾT</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Mã hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tên nhà cung cấp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(4)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tên hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(6)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Đơn vị tính
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(7)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lô hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(8)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số lượng nhập
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(9)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Đơn giá
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(10)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chiết khấu
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(11)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Thành tiền
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(12 = 9*(10-11))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Giảm giá HD
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(13)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Giá trị nhập
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(14 = 12-13)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nhân viên
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(15)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ghi chú
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(16)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mã nhà cung cấp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(3)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiền thuế
-</t>
+    <t>Mã chứng từ</t>
+  </si>
+  <si>
+    <t>Ngày chứng từ</t>
+  </si>
+  <si>
+    <t>Mã nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Tên nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Mã hàng</t>
+  </si>
+  <si>
+    <t>Tên hàng</t>
+  </si>
+  <si>
+    <t>Đơn vị tính</t>
+  </si>
+  <si>
+    <t>Lô hàng</t>
+  </si>
+  <si>
+    <t>Số lượng nhập</t>
+  </si>
+  <si>
+    <t>Đơn giá</t>
+  </si>
+  <si>
+    <t>Chiết khấu</t>
+  </si>
+  <si>
+    <t>Thành tiền</t>
+  </si>
+  <si>
+    <t>Giảm giá HD</t>
+  </si>
+  <si>
+    <t>Giá trị nhập</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Tiền thuế</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Tên  nhóm hàng</t>
   </si>
 </sst>
 </file>
@@ -800,11 +594,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,24 +607,25 @@
     <col min="2" max="2" width="25" style="17" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="17" customWidth="1"/>
     <col min="4" max="4" width="35.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19" style="12" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="7" customWidth="1"/>
-    <col min="16" max="17" width="25.85546875" style="16" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="32.85546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="19" style="12" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="7" customWidth="1"/>
+    <col min="17" max="18" width="25.85546875" style="16" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -848,9 +643,10 @@
       <c r="O1" s="19"/>
       <c r="P1" s="19"/>
       <c r="Q1" s="19"/>
-      <c r="R1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R1" s="19"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -868,8 +664,9 @@
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R2" s="20"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -887,22 +684,23 @@
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
-    </row>
-    <row r="4" spans="1:18" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R3" s="24"/>
+    </row>
+    <row r="4" spans="1:19" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>6</v>
@@ -913,7 +711,7 @@
       <c r="H4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="11" t="s">
@@ -932,16 +730,19 @@
         <v>14</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -950,17 +751,18 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="14"/>
+      <c r="P5" s="6"/>
       <c r="Q5" s="14"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -969,17 +771,18 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="6"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="14"/>
+      <c r="P6" s="6"/>
       <c r="Q6" s="14"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -988,17 +791,18 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="6"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
-      <c r="P7" s="14"/>
+      <c r="P7" s="6"/>
       <c r="Q7" s="14"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -1007,17 +811,18 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="6"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="14"/>
+      <c r="P8" s="6"/>
       <c r="Q8" s="14"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -1026,17 +831,18 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="6"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="14"/>
+      <c r="P9" s="6"/>
       <c r="Q9" s="14"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -1045,17 +851,18 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="6"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="14"/>
+      <c r="P10" s="6"/>
       <c r="Q10" s="14"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -1064,17 +871,18 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="6"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="14"/>
+      <c r="P11" s="6"/>
       <c r="Q11" s="14"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -1083,17 +891,18 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="6"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="14"/>
+      <c r="P12" s="6"/>
       <c r="Q12" s="14"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -1102,17 +911,18 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="6"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
-      <c r="P13" s="14"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="14"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -1121,17 +931,18 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="6"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
-      <c r="P14" s="14"/>
+      <c r="P14" s="6"/>
       <c r="Q14" s="14"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14" s="14"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -1140,17 +951,18 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="6"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
-      <c r="P15" s="14"/>
+      <c r="P15" s="6"/>
       <c r="Q15" s="14"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="14"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -1159,17 +971,18 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="6"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
-      <c r="P16" s="14"/>
+      <c r="P16" s="6"/>
       <c r="Q16" s="14"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="14"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1178,17 +991,18 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="6"/>
+      <c r="I17" s="3"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="14"/>
+      <c r="P17" s="6"/>
       <c r="Q17" s="14"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="14"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -1197,17 +1011,18 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="6"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
-      <c r="P18" s="14"/>
+      <c r="P18" s="6"/>
       <c r="Q18" s="14"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="14"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -1216,17 +1031,18 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="6"/>
+      <c r="I19" s="3"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="P19" s="14"/>
+      <c r="P19" s="6"/>
       <c r="Q19" s="14"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="14"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -1235,17 +1051,18 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="6"/>
+      <c r="I20" s="3"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
-      <c r="P20" s="14"/>
+      <c r="P20" s="6"/>
       <c r="Q20" s="14"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="14"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -1254,17 +1071,18 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="6"/>
+      <c r="I21" s="3"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
-      <c r="P21" s="14"/>
+      <c r="P21" s="6"/>
       <c r="Q21" s="14"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="14"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1273,17 +1091,18 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="6"/>
+      <c r="I22" s="3"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
-      <c r="P22" s="14"/>
+      <c r="P22" s="6"/>
       <c r="Q22" s="14"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="14"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -1292,17 +1111,18 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="6"/>
+      <c r="I23" s="3"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
-      <c r="P23" s="14"/>
+      <c r="P23" s="6"/>
       <c r="Q23" s="14"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -1311,17 +1131,18 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="6"/>
+      <c r="I24" s="3"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
-      <c r="P24" s="14"/>
+      <c r="P24" s="6"/>
       <c r="Q24" s="14"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="14"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -1330,17 +1151,18 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="6"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
-      <c r="P25" s="14"/>
+      <c r="P25" s="6"/>
       <c r="Q25" s="14"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="14"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -1349,17 +1171,18 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="6"/>
+      <c r="I26" s="3"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
-      <c r="P26" s="14"/>
+      <c r="P26" s="6"/>
       <c r="Q26" s="14"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="14"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -1368,17 +1191,18 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="6"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
-      <c r="P27" s="14"/>
+      <c r="P27" s="6"/>
       <c r="Q27" s="14"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="14"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -1387,19 +1211,20 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="6"/>
+      <c r="I28" s="3"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
-      <c r="P28" s="14"/>
+      <c r="P28" s="6"/>
       <c r="Q28" s="14"/>
-    </row>
-    <row r="29" spans="1:17" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R28" s="14"/>
+    </row>
+    <row r="29" spans="1:18" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -1407,17 +1232,14 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="13">
-        <f>SUM(I$5:I28)</f>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="13">
+        <f>SUM(J$5:J28)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="13"/>
       <c r="K29" s="13"/>
-      <c r="L29" s="13">
-        <f>SUM(L$5:L28)</f>
-        <v>0</v>
-      </c>
+      <c r="L29" s="13"/>
       <c r="M29" s="13">
         <f>SUM(M$5:M28)</f>
         <v>0</v>
@@ -1430,15 +1252,19 @@
         <f>SUM(O$5:O28)</f>
         <v>0</v>
       </c>
-      <c r="P29" s="15"/>
+      <c r="P29" s="13">
+        <f>SUM(P$5:P28)</f>
+        <v>0</v>
+      </c>
       <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A3:R3"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>